<commit_message>
Added data cleaning and processing code
</commit_message>
<xml_diff>
--- a/ProjectUpdateInfo.xlsx
+++ b/ProjectUpdateInfo.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae87d82036f066c6/Documents/GitHub/Beyond-The-Headlines-Exploring-Insights-From-Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA81AEB7-38B5-4F28-B43C-F791D70F88A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{DA81AEB7-38B5-4F28-B43C-F791D70F88A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{411A5A11-F541-4136-B823-B40F8C12F401}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BD037917-F868-4D5E-9989-88B5EDAAAF90}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BD037917-F868-4D5E-9989-88B5EDAAAF90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,7 +103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +119,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +158,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -157,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -176,6 +196,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3387,6 +3413,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3686,8 +3716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C007AB3-1CF3-45B1-AF23-E6AFE32B26C0}">
   <dimension ref="A1:S1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="B1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3760,6 +3790,10 @@
         <f>(B2*B2+C2*C2+D2*D2)/SUM(B2:D2)</f>
         <v>74.83226912298737</v>
       </c>
+      <c r="K2">
+        <f>P35</f>
+        <v>0</v>
+      </c>
       <c r="L2">
         <v>2996.84</v>
       </c>
@@ -3797,6 +3831,10 @@
         <f t="shared" ref="J3:J66" si="2">(B3*B3+C3*C3+D3*D3)/SUM(B3:D3)</f>
         <v>75.486342093226469</v>
       </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="3">(0.2*B3+0.2*C3+0.2*D3)</f>
+        <v>42.643199199999998</v>
+      </c>
       <c r="L3">
         <v>3000.77</v>
       </c>
@@ -3822,7 +3860,7 @@
         <v>54.894001000000003</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F67" si="3">F3*B3/B4</f>
+        <f t="shared" ref="F4:F67" si="4">F3*B3/B4</f>
         <v>99.79288347967551</v>
       </c>
       <c r="G4">
@@ -3837,11 +3875,15 @@
         <f t="shared" si="2"/>
         <v>74.763928043438042</v>
       </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>42.115200000000002</v>
+      </c>
       <c r="L4">
         <v>2989.68</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M67" si="4">M3*L4/L3</f>
+        <f t="shared" ref="M4:M67" si="5">M3*L4/L3</f>
         <v>74.653481117314527</v>
       </c>
     </row>
@@ -3859,7 +3901,7 @@
         <v>59.346001000000001</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.785729416695219</v>
       </c>
       <c r="G5">
@@ -3874,11 +3916,15 @@
         <f t="shared" si="2"/>
         <v>79.18200123013392</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>44.968600400000007</v>
+      </c>
       <c r="L5">
         <v>2973.61</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.252206920224793</v>
       </c>
       <c r="N5" s="5" t="s">
@@ -3910,7 +3956,7 @@
         <v>59.325499999999998</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>92.861277195737628</v>
       </c>
       <c r="G6">
@@ -3925,11 +3971,15 @@
         <f t="shared" si="2"/>
         <v>79.382935800776835</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>44.952600000000004</v>
+      </c>
       <c r="L6">
         <v>2965.81</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.057437863765557</v>
       </c>
       <c r="N6" s="6"/>
@@ -3953,7 +4003,7 @@
         <v>60.514000000000003</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90.543840627087889</v>
       </c>
       <c r="G7">
@@ -3968,11 +4018,15 @@
         <f t="shared" si="2"/>
         <v>80.814310289716943</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>45.836300800000004</v>
+      </c>
       <c r="L7">
         <v>2963.07</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.989018990086294</v>
       </c>
       <c r="N7" s="5" t="s">
@@ -3998,7 +4052,7 @@
         <v>60.572498000000003</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89.89514951737452</v>
       </c>
       <c r="G8">
@@ -4013,11 +4067,15 @@
         <f t="shared" si="2"/>
         <v>80.928237675365949</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>45.941599199999999</v>
+      </c>
       <c r="L8">
         <v>2918.55</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.877337144757419</v>
       </c>
       <c r="N8" s="7" t="s">
@@ -4049,7 +4107,7 @@
         <v>60.877997999999998</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88.164685818847218</v>
       </c>
       <c r="G9">
@@ -4064,11 +4122,15 @@
         <f t="shared" si="2"/>
         <v>84.721549786372179</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>47.526798999999997</v>
+      </c>
       <c r="L9">
         <v>2911.1</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.69130772544699</v>
       </c>
       <c r="N9" s="7" t="s">
@@ -4094,7 +4156,7 @@
         <v>63.461497999999999</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.926150172840281</v>
       </c>
       <c r="G10">
@@ -4109,11 +4171,15 @@
         <f t="shared" si="2"/>
         <v>89.061685333764132</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>49.877999000000003</v>
+      </c>
       <c r="L10">
         <v>2920.4</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.923532369686853</v>
       </c>
       <c r="N10" s="7" t="s">
@@ -4139,7 +4205,7 @@
         <v>63.123500999999997</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>84.69922679602648</v>
       </c>
       <c r="G11">
@@ -4154,11 +4220,15 @@
         <f t="shared" si="2"/>
         <v>89.555197482164999</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>49.923000399999999</v>
+      </c>
       <c r="L11">
         <v>2944.23</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.518576807561686</v>
       </c>
       <c r="N11" s="7"/>
@@ -4182,7 +4252,7 @@
         <v>63.173499999999997</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>84.031532539934673</v>
       </c>
       <c r="G12">
@@ -4197,11 +4267,15 @@
         <f t="shared" si="2"/>
         <v>92.559361500675351</v>
       </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>51.0511002</v>
+      </c>
       <c r="L12">
         <v>2918.56</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.877586848675961</v>
       </c>
       <c r="N12" s="6"/>
@@ -4225,7 +4299,7 @@
         <v>64.162497999999999</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>85.18741662747172</v>
       </c>
       <c r="G13">
@@ -4240,11 +4314,15 @@
         <f t="shared" si="2"/>
         <v>91.544693905558617</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>50.722498999999999</v>
+      </c>
       <c r="L13">
         <v>2885.38</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.0490692469686</v>
       </c>
       <c r="N13" s="5" t="s">
@@ -4270,7 +4348,7 @@
         <v>63.330502000000003</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>86.993106907683725</v>
       </c>
       <c r="G14">
@@ -4285,11 +4363,15 @@
         <f t="shared" si="2"/>
         <v>91.686456746928457</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>50.448699200000007</v>
+      </c>
       <c r="L14">
         <v>2924.78</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.032902686006295</v>
       </c>
       <c r="N14" s="1"/>
@@ -4313,7 +4395,7 @@
         <v>60.817000999999998</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>89.767860636700973</v>
       </c>
       <c r="G15">
@@ -4328,11 +4410,15 @@
         <f t="shared" si="2"/>
         <v>89.026146851621363</v>
       </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>48.863099599999998</v>
+      </c>
       <c r="L15">
         <v>2983.69</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.503908470110602</v>
       </c>
       <c r="N15" s="1"/>
@@ -4356,7 +4442,7 @@
         <v>63.160499999999999</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87.254616812615239</v>
       </c>
       <c r="G16">
@@ -4371,11 +4457,15 @@
         <f t="shared" si="2"/>
         <v>90.744974956502844</v>
       </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>50.0720004</v>
+      </c>
       <c r="L16">
         <v>2967.07</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.088900557501304</v>
       </c>
       <c r="N16" s="1"/>
@@ -4399,7 +4489,7 @@
         <v>63.815497999999998</v>
       </c>
       <c r="F17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87.594082100134543</v>
       </c>
       <c r="G17">
@@ -4414,11 +4504,15 @@
         <f t="shared" si="2"/>
         <v>91.838552354292247</v>
       </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>50.509100400000008</v>
+      </c>
       <c r="L17">
         <v>2985.47</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.548355767610275</v>
       </c>
       <c r="N17" s="1" t="s">
@@ -4444,7 +4538,7 @@
         <v>63.965499999999999</v>
       </c>
       <c r="F18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>85.136234936565714</v>
       </c>
       <c r="G18">
@@ -4459,11 +4553,15 @@
         <f t="shared" si="2"/>
         <v>92.544003050149087</v>
       </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>51.043800400000002</v>
+      </c>
       <c r="L18">
         <v>2985.73</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.554848069492252</v>
       </c>
     </row>
@@ -4481,26 +4579,30 @@
         <v>63.793998999999999</v>
       </c>
       <c r="F19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>85.076100501772061</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G82" si="5">G18*C18/C19</f>
+        <f t="shared" ref="G19:G82" si="6">G18*C18/C19</f>
         <v>80.290403696370277</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:H82" si="6">H18*D18/D19</f>
+        <f t="shared" ref="H19:H82" si="7">H18*D18/D19</f>
         <v>86.655483065107745</v>
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
         <v>91.538787759107464</v>
       </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>50.677301</v>
+      </c>
       <c r="L19">
         <v>2968.35</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.120862659074106</v>
       </c>
     </row>
@@ -4518,26 +4620,30 @@
         <v>61.683498</v>
       </c>
       <c r="F20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>86.47785712446796</v>
       </c>
       <c r="G20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>82.438809679201938</v>
       </c>
       <c r="H20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>89.620400581043569</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
         <v>89.229942939296834</v>
       </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>49.406499400000008</v>
+      </c>
       <c r="L20">
         <v>3002.43</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.971853613449852</v>
       </c>
     </row>
@@ -4555,26 +4661,30 @@
         <v>67.073997000000006</v>
       </c>
       <c r="F21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.727798266661182</v>
       </c>
       <c r="G21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80.401737766549445</v>
       </c>
       <c r="H21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>82.417927173774956</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
         <v>92.172812008347421</v>
       </c>
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>51.5283996</v>
+      </c>
       <c r="L21">
         <v>2983.5</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.499164095658401</v>
       </c>
     </row>
@@ -4592,26 +4702,30 @@
         <v>67.432998999999995</v>
       </c>
       <c r="F22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>81.997962505022301</v>
       </c>
       <c r="G22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77.109946898381907</v>
       </c>
       <c r="H22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>81.979147924297422</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
         <v>95.409763057726153</v>
       </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>52.9165986</v>
+      </c>
       <c r="L22">
         <v>3008.42</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.121426260653806</v>
       </c>
     </row>
@@ -4629,26 +4743,30 @@
         <v>66.030501999999998</v>
       </c>
       <c r="F23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>83.339674588447807</v>
       </c>
       <c r="G23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>83.449983666952747</v>
       </c>
       <c r="H23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>83.720396370756049</v>
       </c>
       <c r="J23">
         <f t="shared" si="2"/>
         <v>89.657823289600444</v>
       </c>
+      <c r="K23">
+        <f t="shared" si="3"/>
+        <v>50.520001199999996</v>
+      </c>
       <c r="L23">
         <v>3010.36</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.169868820850084</v>
       </c>
     </row>
@@ -4666,26 +4784,30 @@
         <v>66.339995999999999</v>
       </c>
       <c r="F24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>82.176968451671868</v>
       </c>
       <c r="G24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>82.370823708219817</v>
       </c>
       <c r="H24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>83.32981810852084</v>
       </c>
       <c r="J24">
         <f t="shared" si="2"/>
         <v>90.756720693499304</v>
       </c>
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>51.085899400000002</v>
+      </c>
       <c r="L24">
         <v>3001.5</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.948631149025871</v>
       </c>
     </row>
@@ -4703,26 +4825,30 @@
         <v>67.555496000000005</v>
       </c>
       <c r="F25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80.961825258258173</v>
       </c>
       <c r="G25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>82.306499976758133</v>
       </c>
       <c r="H25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>81.83049681109587</v>
       </c>
       <c r="J25">
         <f t="shared" si="2"/>
         <v>91.252404757143395</v>
       </c>
+      <c r="K25">
+        <f t="shared" si="3"/>
+        <v>51.567098800000011</v>
+      </c>
       <c r="L25">
         <v>2995.67</v>
       </c>
       <c r="M25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.803053764518523</v>
       </c>
     </row>
@@ -4740,26 +4866,30 @@
         <v>67.364998</v>
       </c>
       <c r="F26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80.135049993213585</v>
       </c>
       <c r="G26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>81.135220056132624</v>
       </c>
       <c r="H26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>82.061901048375304</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
         <v>92.307154934387171</v>
       </c>
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>52.017100599999999</v>
+      </c>
       <c r="L26">
         <v>2996.41</v>
       </c>
       <c r="M26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.821531854490303</v>
       </c>
     </row>
@@ -4777,26 +4907,30 @@
         <v>68.627998000000005</v>
       </c>
       <c r="F27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79.314548740753239</v>
       </c>
       <c r="G27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80.574926777848333</v>
       </c>
       <c r="H27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80.551669305579907</v>
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
         <v>93.137382468747688</v>
       </c>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>52.588699400000003</v>
+      </c>
       <c r="L27">
         <v>3012.21</v>
       </c>
       <c r="M27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.216064045779532</v>
       </c>
     </row>
@@ -4814,26 +4948,30 @@
         <v>69.418503000000001</v>
       </c>
       <c r="F28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77.680327892427968</v>
       </c>
       <c r="G28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80.168601410891725</v>
       </c>
       <c r="H28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>79.634385086062721</v>
       </c>
       <c r="J28">
         <f t="shared" si="2"/>
         <v>93.958692860713896</v>
       </c>
+      <c r="K28">
+        <f t="shared" si="3"/>
+        <v>53.186300599999996</v>
+      </c>
       <c r="L28">
         <v>3009.08</v>
       </c>
       <c r="M28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.137906719277296</v>
       </c>
     </row>
@@ -4851,26 +4989,30 @@
         <v>70.163002000000006</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76.476936567678806</v>
       </c>
       <c r="G29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79.190539124712473</v>
       </c>
       <c r="H29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.789385323051022</v>
       </c>
       <c r="J29">
         <f t="shared" si="2"/>
         <v>95.160683543554512</v>
       </c>
+      <c r="K29">
+        <f t="shared" si="3"/>
+        <v>53.873100200000003</v>
+      </c>
       <c r="L29">
         <v>2981.41</v>
       </c>
       <c r="M29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.446975976684072</v>
       </c>
     </row>
@@ -4888,26 +5030,30 @@
         <v>68.787002999999999</v>
       </c>
       <c r="F30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77.361035581888345</v>
       </c>
       <c r="G30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80.939348532999063</v>
       </c>
       <c r="H30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80.36546962221918</v>
       </c>
       <c r="J30">
         <f t="shared" si="2"/>
         <v>93.315350645529733</v>
       </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>52.897401599999995</v>
+      </c>
       <c r="L30">
         <v>2971.01</v>
       </c>
       <c r="M30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.187283901405095</v>
       </c>
     </row>
@@ -4925,26 +5071,30 @@
         <v>67.466498999999999</v>
       </c>
       <c r="F31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78.306520482535859</v>
       </c>
       <c r="G31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>80.56437614228939</v>
       </c>
       <c r="H31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>81.938441773894311</v>
       </c>
       <c r="J31">
         <f t="shared" si="2"/>
         <v>93.178097253950824</v>
       </c>
+      <c r="K31">
+        <f t="shared" si="3"/>
+        <v>52.555000200000009</v>
+      </c>
       <c r="L31">
         <v>2988.43</v>
       </c>
       <c r="M31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.622268127497378</v>
       </c>
     </row>
@@ -4962,26 +5112,30 @@
         <v>67.806503000000006</v>
       </c>
       <c r="F32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77.828389795738431</v>
       </c>
       <c r="G32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79.858513004797615</v>
       </c>
       <c r="H32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>81.52757560731304</v>
       </c>
       <c r="J32">
         <f t="shared" si="2"/>
         <v>93.913368219492909</v>
       </c>
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>52.926800400000005</v>
+      </c>
       <c r="L32">
         <v>2980.33</v>
       </c>
       <c r="M32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.420007953482013</v>
       </c>
     </row>
@@ -4999,26 +5153,30 @@
         <v>68.659499999999994</v>
       </c>
       <c r="F33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78.291251588606173</v>
       </c>
       <c r="G33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79.164905994155589</v>
       </c>
       <c r="H33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80.514711001390921</v>
       </c>
       <c r="J33">
         <f t="shared" si="2"/>
         <v>94.520234466524414</v>
       </c>
+      <c r="K33">
+        <f t="shared" si="3"/>
+        <v>53.215199200000001</v>
+      </c>
       <c r="L33">
         <v>2960.6</v>
       </c>
       <c r="M33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.927342122207563</v>
       </c>
     </row>
@@ -5036,26 +5194,30 @@
         <v>69.196999000000005</v>
       </c>
       <c r="F34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76.489081190985019</v>
       </c>
       <c r="G34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78.627186579272248</v>
       </c>
       <c r="H34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>79.889299823537129</v>
       </c>
       <c r="J34">
         <f t="shared" si="2"/>
         <v>95.469106034098118</v>
       </c>
+      <c r="K34">
+        <f t="shared" si="3"/>
+        <v>53.850000200000004</v>
+      </c>
       <c r="L34">
         <v>2924.67</v>
       </c>
       <c r="M34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.030155942902397</v>
       </c>
     </row>
@@ -5073,26 +5235,30 @@
         <v>68.674248000000006</v>
       </c>
       <c r="F35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76.93363725190585</v>
       </c>
       <c r="G35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77.886607993913501</v>
       </c>
       <c r="H35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>80.497420226574576</v>
       </c>
       <c r="J35">
         <f t="shared" si="2"/>
         <v>95.91784553274762</v>
       </c>
+      <c r="K35">
+        <f t="shared" si="3"/>
+        <v>53.885150200000005</v>
+      </c>
       <c r="L35">
         <v>2909.01</v>
       </c>
       <c r="M35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.639119606472704</v>
       </c>
     </row>
@@ -5110,26 +5276,30 @@
         <v>70.335999000000001</v>
       </c>
       <c r="F36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.465963394444231</v>
       </c>
       <c r="G36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76.370929412933961</v>
       </c>
       <c r="H36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.595596545092064</v>
       </c>
       <c r="J36">
         <f t="shared" si="2"/>
         <v>97.860682915794598</v>
       </c>
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>55.008100999999996</v>
+      </c>
       <c r="L36">
         <v>2937.09</v>
       </c>
       <c r="M36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.340288209725955</v>
       </c>
     </row>
@@ -5147,26 +5317,30 @@
         <v>70.139999000000003</v>
       </c>
       <c r="F37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76.032822445123585</v>
       </c>
       <c r="G37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77.969055608181591</v>
       </c>
       <c r="H37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.815224961722606</v>
       </c>
       <c r="J37">
         <f t="shared" si="2"/>
         <v>96.288524616374687</v>
       </c>
+      <c r="K37">
+        <f t="shared" si="3"/>
+        <v>54.337899800000002</v>
+      </c>
       <c r="L37">
         <v>2910.37</v>
       </c>
       <c r="M37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.673079339393794</v>
       </c>
     </row>
@@ -5184,26 +5358,30 @@
         <v>70.521004000000005</v>
       </c>
       <c r="F38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.546424131384484</v>
       </c>
       <c r="G38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78.284528113250914</v>
       </c>
       <c r="H38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.389408636326266</v>
       </c>
       <c r="J38">
         <f t="shared" si="2"/>
         <v>96.200117648083292</v>
       </c>
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>54.417501999999999</v>
+      </c>
       <c r="L38">
         <v>2861.28</v>
       </c>
       <c r="M38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.447282803293291</v>
       </c>
     </row>
@@ -5221,26 +5399,30 @@
         <v>70.850998000000004</v>
       </c>
       <c r="F39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76.061628160453523</v>
       </c>
       <c r="G39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78.770036603766755</v>
       </c>
       <c r="H39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.024303906064944</v>
       </c>
       <c r="J39">
         <f t="shared" si="2"/>
         <v>95.723758264654109</v>
       </c>
+      <c r="K39">
+        <f t="shared" si="3"/>
+        <v>54.225300600000004</v>
+      </c>
       <c r="L39">
         <v>2893.14</v>
       </c>
       <c r="M39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.242839487753713</v>
       </c>
     </row>
@@ -5258,26 +5440,30 @@
         <v>70.891998000000001</v>
       </c>
       <c r="F40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.731670213783616</v>
       </c>
       <c r="G40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79.144869675489275</v>
       </c>
       <c r="H40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77.979178975883855</v>
       </c>
       <c r="J40">
         <f t="shared" si="2"/>
         <v>95.50211892441331</v>
       </c>
+      <c r="K40">
+        <f t="shared" si="3"/>
+        <v>54.187799000000005</v>
+      </c>
       <c r="L40">
         <v>2866.7</v>
       </c>
       <c r="M40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.582622327140598</v>
       </c>
     </row>
@@ -5295,26 +5481,30 @@
         <v>70.836501999999996</v>
       </c>
       <c r="F41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.698351610369158</v>
       </c>
       <c r="G41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79.451086585315068</v>
       </c>
       <c r="H41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.040270819696886</v>
       </c>
       <c r="J41">
         <f t="shared" si="2"/>
         <v>95.25170364033292</v>
       </c>
+      <c r="K41">
+        <f t="shared" si="3"/>
+        <v>54.090800400000006</v>
+      </c>
       <c r="L41">
         <v>2911.07</v>
       </c>
       <c r="M41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.690558613691422</v>
       </c>
     </row>
@@ -5332,26 +5522,30 @@
         <v>71.445999</v>
       </c>
       <c r="F42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75.772158573665948</v>
       </c>
       <c r="G42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>78.108560128072327</v>
       </c>
       <c r="H42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77.374518900631514</v>
       </c>
       <c r="J42">
         <f t="shared" si="2"/>
         <v>96.448901020979733</v>
       </c>
+      <c r="K42">
+        <f t="shared" si="3"/>
+        <v>54.609900000000003</v>
+      </c>
       <c r="L42">
         <v>2930.94</v>
       </c>
       <c r="M42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.18672029982541</v>
       </c>
     </row>
@@ -5369,26 +5563,30 @@
         <v>71.591003000000001</v>
       </c>
       <c r="F43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74.85163834452969</v>
       </c>
       <c r="G43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77.202311946349525</v>
       </c>
       <c r="H43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77.217800678110351</v>
       </c>
       <c r="J43">
         <f t="shared" si="2"/>
         <v>97.474769025039905</v>
       </c>
+      <c r="K43">
+        <f t="shared" si="3"/>
+        <v>55.121101400000001</v>
+      </c>
       <c r="L43">
         <v>2922.04</v>
       </c>
       <c r="M43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.964483812327046</v>
       </c>
     </row>
@@ -5406,26 +5604,30 @@
         <v>71.960999000000001</v>
       </c>
       <c r="F44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74.506713360632276</v>
       </c>
       <c r="G44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77.159534843812594</v>
       </c>
       <c r="H44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.820776209624327</v>
       </c>
       <c r="J44">
         <f t="shared" si="2"/>
         <v>97.659548204957545</v>
       </c>
+      <c r="K44">
+        <f t="shared" si="3"/>
+        <v>55.283299400000004</v>
+      </c>
       <c r="L44">
         <v>2919.01</v>
       </c>
       <c r="M44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.888823525010196</v>
       </c>
     </row>
@@ -5443,26 +5645,30 @@
         <v>71.819000000000003</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74.09879643330207</v>
       </c>
       <c r="G45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76.973049983425597</v>
       </c>
       <c r="H45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.972664615213247</v>
       </c>
       <c r="J45">
         <f t="shared" si="2"/>
         <v>97.901491220690559</v>
       </c>
+      <c r="K45">
+        <f t="shared" si="3"/>
+        <v>55.403799399999997</v>
+      </c>
       <c r="L45">
         <v>2913.48</v>
       </c>
       <c r="M45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.750737258058962</v>
       </c>
     </row>
@@ -5480,26 +5686,30 @@
         <v>70.609001000000006</v>
       </c>
       <c r="F46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74.74249131937222</v>
       </c>
       <c r="G46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77.529873019018723</v>
       </c>
       <c r="H46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.291715244632911</v>
       </c>
       <c r="J46">
         <f t="shared" si="2"/>
         <v>97.058001831973712</v>
       </c>
+      <c r="K46">
+        <f t="shared" si="3"/>
+        <v>54.843800400000006</v>
+      </c>
       <c r="L46">
         <v>2864.74</v>
       </c>
       <c r="M46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.533680359107251</v>
       </c>
     </row>
@@ -5517,26 +5727,30 @@
         <v>71.919501999999994</v>
       </c>
       <c r="F47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72.672701055806883</v>
       </c>
       <c r="G47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76.830447413122073</v>
       </c>
       <c r="H47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.865101207180231</v>
       </c>
       <c r="J47">
         <f t="shared" si="2"/>
         <v>98.420664310805023</v>
       </c>
+      <c r="K47">
+        <f t="shared" si="3"/>
+        <v>55.788900800000008</v>
+      </c>
       <c r="L47">
         <v>2846.2</v>
       </c>
       <c r="M47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.070729294138758</v>
       </c>
     </row>
@@ -5554,26 +5768,30 @@
         <v>72.330498000000006</v>
       </c>
       <c r="F48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72.245549625035622</v>
       </c>
       <c r="G48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75.580611976404398</v>
       </c>
       <c r="H48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.428338707138451</v>
       </c>
       <c r="J48">
         <f t="shared" si="2"/>
         <v>99.711853374167887</v>
       </c>
+      <c r="K48">
+        <f t="shared" si="3"/>
+        <v>56.379699800000004</v>
+      </c>
       <c r="L48">
         <v>2894.15</v>
       </c>
       <c r="M48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.268059583525996</v>
       </c>
     </row>
@@ -5591,26 +5809,30 @@
         <v>72.807998999999995</v>
       </c>
       <c r="F49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70.034015408215666</v>
       </c>
       <c r="G49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>73.348817493819865</v>
       </c>
       <c r="H49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75.927094219414016</v>
       </c>
       <c r="J49">
         <f t="shared" si="2"/>
         <v>102.50271813621632</v>
       </c>
+      <c r="K49">
+        <f t="shared" si="3"/>
+        <v>57.769699200000005</v>
+      </c>
       <c r="L49">
         <v>2880.72</v>
       </c>
       <c r="M49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.932707220930155</v>
       </c>
     </row>
@@ -5628,26 +5850,30 @@
         <v>73.292502999999996</v>
       </c>
       <c r="F50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.277408097465184</v>
       </c>
       <c r="G50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72.058020692485528</v>
       </c>
       <c r="H50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75.425174113647088</v>
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
         <v>104.38204388377717</v>
       </c>
+      <c r="K50">
+        <f t="shared" si="3"/>
+        <v>58.775000000000006</v>
+      </c>
       <c r="L50">
         <v>2907.07</v>
       </c>
       <c r="M50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.59067704627644</v>
       </c>
     </row>
@@ -5665,26 +5891,30 @@
         <v>70.192001000000005</v>
       </c>
       <c r="F51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71.720753122256653</v>
       </c>
       <c r="G51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>74.578961174241329</v>
       </c>
       <c r="H51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.756834414793232</v>
       </c>
       <c r="J51">
         <f t="shared" si="2"/>
         <v>100.46129886355776</v>
       </c>
+      <c r="K51">
+        <f t="shared" si="3"/>
+        <v>56.413000400000001</v>
+      </c>
       <c r="L51">
         <v>2930.51</v>
       </c>
       <c r="M51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.1759830313283</v>
       </c>
     </row>
@@ -5702,26 +5932,30 @@
         <v>70.658996999999999</v>
       </c>
       <c r="F52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71.106851396936847</v>
       </c>
       <c r="G52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>74.958155731256781</v>
       </c>
       <c r="H52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.23631858233145</v>
       </c>
       <c r="J52">
         <f t="shared" si="2"/>
         <v>100.34889352035057</v>
       </c>
+      <c r="K52">
+        <f t="shared" si="3"/>
+        <v>56.521998599999996</v>
+      </c>
       <c r="L52">
         <v>2896.21</v>
       </c>
       <c r="M52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.319498590744729</v>
       </c>
     </row>
@@ -5739,26 +5973,30 @@
         <v>70.992500000000007</v>
       </c>
       <c r="F53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70.238202168884243</v>
       </c>
       <c r="G53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>74.152245732413377</v>
       </c>
       <c r="H53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77.868786139380944</v>
       </c>
       <c r="J53">
         <f t="shared" si="2"/>
         <v>101.40824004956924</v>
       </c>
+      <c r="K53">
+        <f t="shared" si="3"/>
+        <v>57.074800200000006</v>
+      </c>
       <c r="L53">
         <v>2858.65</v>
       </c>
       <c r="M53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.38161067271794</v>
       </c>
     </row>
@@ -5776,26 +6014,30 @@
         <v>72.136002000000005</v>
       </c>
       <c r="F54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.424793288734108</v>
       </c>
       <c r="G54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72.944666579139692</v>
       </c>
       <c r="H54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.634407878606879</v>
       </c>
       <c r="J54">
         <f t="shared" si="2"/>
         <v>103.2939226311755</v>
       </c>
+      <c r="K54">
+        <f t="shared" si="3"/>
+        <v>58.183900600000015</v>
+      </c>
       <c r="L54">
         <v>2861.18</v>
       </c>
       <c r="M54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.44478576410792</v>
       </c>
     </row>
@@ -5813,26 +6055,30 @@
         <v>72.555999999999997</v>
       </c>
       <c r="F55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.520153229843288</v>
       </c>
       <c r="G55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>72.234552998797511</v>
       </c>
       <c r="H55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.190801587739159</v>
       </c>
       <c r="J55">
         <f t="shared" si="2"/>
         <v>104.02400434588778</v>
       </c>
+      <c r="K55">
+        <f t="shared" si="3"/>
+        <v>58.500499000000005</v>
+      </c>
       <c r="L55">
         <v>2898.07</v>
       </c>
       <c r="M55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>72.365943519592719</v>
       </c>
     </row>
@@ -5850,26 +6096,30 @@
         <v>71.797996999999995</v>
       </c>
       <c r="F56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.492876860334533</v>
       </c>
       <c r="G56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71.880721336230067</v>
       </c>
       <c r="H56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.995181355825324</v>
       </c>
       <c r="J56">
         <f t="shared" si="2"/>
         <v>104.28531616550471</v>
       </c>
+      <c r="K56">
+        <f t="shared" si="3"/>
+        <v>58.485901000000005</v>
+      </c>
       <c r="L56">
         <v>2943.9</v>
       </c>
       <c r="M56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>73.510336578250005</v>
       </c>
     </row>
@@ -5887,26 +6137,30 @@
         <v>71.585999000000001</v>
       </c>
       <c r="F57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.886538945442027</v>
       </c>
       <c r="G57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71.315620612539902</v>
       </c>
       <c r="H57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77.22319835195708</v>
       </c>
       <c r="J57">
         <f t="shared" si="2"/>
         <v>104.71743576853811</v>
       </c>
+      <c r="K57">
+        <f t="shared" si="3"/>
+        <v>58.5533006</v>
+      </c>
       <c r="L57">
         <v>2980.32</v>
       </c>
       <c r="M57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.419758249563515</v>
       </c>
     </row>
@@ -5924,26 +6178,30 @@
         <v>72.593001999999998</v>
       </c>
       <c r="F58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67.130160416085559</v>
       </c>
       <c r="G58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>70.29575006282289</v>
       </c>
       <c r="H58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.15196572253619</v>
       </c>
       <c r="J58">
         <f t="shared" si="2"/>
         <v>106.47939675233859</v>
       </c>
+      <c r="K58">
+        <f t="shared" si="3"/>
+        <v>59.600298999999993</v>
+      </c>
       <c r="L58">
         <v>3016.22</v>
       </c>
       <c r="M58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.31619531711307</v>
       </c>
     </row>
@@ -5961,26 +6219,30 @@
         <v>73.220496999999995</v>
       </c>
       <c r="F59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65.727226693585749</v>
       </c>
       <c r="G59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69.009299307653379</v>
       </c>
       <c r="H59">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75.499348222124212</v>
       </c>
       <c r="J59">
         <f t="shared" si="2"/>
         <v>108.43133438842185</v>
       </c>
+      <c r="K59">
+        <f t="shared" si="3"/>
+        <v>60.614700400000004</v>
+      </c>
       <c r="L59">
         <v>3007.66</v>
       </c>
       <c r="M59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.102448762844986</v>
       </c>
     </row>
@@ -5998,26 +6260,30 @@
         <v>71.598502999999994</v>
       </c>
       <c r="F60">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.908294916494924</v>
       </c>
       <c r="G60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69.766677371513481</v>
       </c>
       <c r="H60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77.209712052219885</v>
       </c>
       <c r="J60">
         <f t="shared" si="2"/>
         <v>106.99905987511906</v>
       </c>
+      <c r="K60">
+        <f t="shared" si="3"/>
+        <v>59.666700599999999</v>
+      </c>
       <c r="L60">
         <v>3024.47</v>
       </c>
       <c r="M60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.522201049906499</v>
       </c>
     </row>
@@ -6035,26 +6301,30 @@
         <v>72.066497999999996</v>
       </c>
       <c r="F61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.031686942568612</v>
       </c>
       <c r="G61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69.255566532667302</v>
       </c>
       <c r="H61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.708317365442142</v>
       </c>
       <c r="J61">
         <f t="shared" si="2"/>
         <v>107.91205637931522</v>
       </c>
+      <c r="K61">
+        <f t="shared" si="3"/>
+        <v>60.201100199999999</v>
+      </c>
       <c r="L61">
         <v>3013.25</v>
       </c>
       <c r="M61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.242033253307454</v>
       </c>
     </row>
@@ -6072,26 +6342,30 @@
         <v>67.995002999999997</v>
       </c>
       <c r="F62">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>68.124876643668458</v>
       </c>
       <c r="G62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>70.842637223897356</v>
       </c>
       <c r="H62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>81.301559763149086</v>
       </c>
       <c r="J62">
         <f t="shared" si="2"/>
         <v>105.02833693855858</v>
       </c>
+      <c r="K62">
+        <f t="shared" si="3"/>
+        <v>58.209199600000005</v>
+      </c>
       <c r="L62">
         <v>3016.26</v>
       </c>
       <c r="M62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.317194132787236</v>
       </c>
     </row>
@@ -6109,26 +6383,30 @@
         <v>69.748497</v>
       </c>
       <c r="F63">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.590194040577103</v>
       </c>
       <c r="G63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>71.172747248660571</v>
       </c>
       <c r="H63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>79.257618984965376</v>
       </c>
       <c r="J63">
         <f t="shared" si="2"/>
         <v>105.38723897852218</v>
       </c>
+      <c r="K63">
+        <f t="shared" si="3"/>
+        <v>58.842498800000001</v>
+      </c>
       <c r="L63">
         <v>2998.77</v>
       </c>
       <c r="M63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.880461979265164</v>
       </c>
     </row>
@@ -6146,26 +6424,30 @@
         <v>70.680496000000005</v>
       </c>
       <c r="F64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.038928707420851</v>
       </c>
       <c r="G64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69.149133433096765</v>
       </c>
       <c r="H64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78.21252131563989</v>
       </c>
       <c r="J64">
         <f t="shared" si="2"/>
         <v>107.86715160716302</v>
       </c>
+      <c r="K64">
+        <f t="shared" si="3"/>
+        <v>59.964297400000007</v>
+      </c>
       <c r="L64">
         <v>2994.74</v>
       </c>
       <c r="M64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.779831300094557</v>
       </c>
     </row>
@@ -6183,26 +6465,30 @@
         <v>71.902000000000001</v>
       </c>
       <c r="F65">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.164075303136926</v>
       </c>
       <c r="G65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66.269498958133852</v>
       </c>
       <c r="H65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76.883811298712132</v>
       </c>
       <c r="J65">
         <f t="shared" si="2"/>
         <v>111.36246437585582</v>
       </c>
+      <c r="K65">
+        <f t="shared" si="3"/>
+        <v>61.372898800000009</v>
+      </c>
       <c r="L65">
         <v>2981.93</v>
       </c>
       <c r="M65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.45996058044804</v>
       </c>
     </row>
@@ -6220,26 +6506,30 @@
         <v>73.235000999999997</v>
       </c>
       <c r="F66">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>66.164075303136926</v>
       </c>
       <c r="G66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66.003530886091625</v>
       </c>
       <c r="H66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>75.484395774091681</v>
       </c>
       <c r="J66">
         <f t="shared" si="2"/>
         <v>111.84090739394432</v>
       </c>
+      <c r="K66">
+        <f t="shared" si="3"/>
+        <v>61.755499200000003</v>
+      </c>
       <c r="L66">
         <v>3004.26</v>
       </c>
       <c r="M66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75.017549430542246</v>
       </c>
     </row>
@@ -6257,26 +6547,30 @@
         <v>74.785004000000001</v>
       </c>
       <c r="F67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>64.440283227170568</v>
       </c>
       <c r="G67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>62.403500693366773</v>
       </c>
       <c r="H67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>73.919897095947206</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J86" si="7">(B67*B67+C67*C67+D67*D67)/SUM(B67:D67)</f>
+        <f t="shared" ref="J67:J86" si="8">(B67*B67+C67*C67+D67*D67)/SUM(B67:D67)</f>
         <v>117.38345978328208</v>
+      </c>
+      <c r="K67">
+        <f t="shared" ref="K67:K86" si="9">(0.2*B67+0.2*C67+0.2*D67)</f>
+        <v>64.219902200000007</v>
       </c>
       <c r="L67">
         <v>2978.87</v>
       </c>
       <c r="M67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74.383551181375566</v>
       </c>
     </row>
@@ -6294,26 +6588,30 @@
         <v>74.259003000000007</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F86" si="8">F67*B67/B68</f>
+        <f t="shared" ref="F68:F86" si="10">F67*B67/B68</f>
         <v>64.640854708837281</v>
       </c>
       <c r="G68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>63.587459106718249</v>
       </c>
       <c r="H68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>74.443496097032153</v>
       </c>
       <c r="J68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>115.60484659029943</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="9"/>
+        <v>63.487500200000014</v>
       </c>
       <c r="L68">
         <v>3005.1</v>
       </c>
       <c r="M68">
-        <f t="shared" ref="M68:M131" si="9">M67*L68/L67</f>
+        <f t="shared" ref="M68:M86" si="11">M67*L68/L67</f>
         <v>75.038524559699397</v>
       </c>
     </row>
@@ -6331,26 +6629,30 @@
         <v>74.800003000000004</v>
       </c>
       <c r="F69">
+        <f t="shared" si="10"/>
+        <v>63.169627009671686</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="6"/>
+        <v>61.916000711847374</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="7"/>
+        <v>73.905074575999663</v>
+      </c>
+      <c r="J69">
         <f t="shared" si="8"/>
-        <v>63.169627009671686</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="5"/>
-        <v>61.916000711847374</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="6"/>
-        <v>73.905074575999663</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="7"/>
         <v>118.50267012497416</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="9"/>
+        <v>64.8395996</v>
       </c>
       <c r="L69">
         <v>3012.13</v>
       </c>
       <c r="M69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>75.214066414431244</v>
       </c>
     </row>
@@ -6368,26 +6670,30 @@
         <v>75.549499999999995</v>
       </c>
       <c r="F70">
+        <f t="shared" si="10"/>
+        <v>62.899140745168154</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="6"/>
+        <v>59.940993455098464</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="7"/>
+        <v>73.171891276580254</v>
+      </c>
+      <c r="J70">
         <f t="shared" si="8"/>
-        <v>62.899140745168154</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="5"/>
-        <v>59.940993455098464</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="6"/>
-        <v>73.171891276580254</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="7"/>
         <v>121.65565125342528</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="9"/>
+        <v>66.086700399999998</v>
       </c>
       <c r="L70">
         <v>3017.8</v>
       </c>
       <c r="M70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>75.355648536242001</v>
       </c>
     </row>
@@ -6405,26 +6711,30 @@
         <v>77.086997999999994</v>
       </c>
       <c r="F71">
+        <f t="shared" si="10"/>
+        <v>62.789305938058874</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="6"/>
+        <v>59.615626250000005</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="7"/>
+        <v>71.712479969709037</v>
+      </c>
+      <c r="J71">
         <f t="shared" si="8"/>
-        <v>62.789305938058874</v>
-      </c>
-      <c r="G71">
-        <f t="shared" si="5"/>
-        <v>59.615626250000005</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="6"/>
-        <v>71.712479969709037</v>
-      </c>
-      <c r="J71">
-        <f t="shared" si="7"/>
         <v>122.34893490637658</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="9"/>
+        <v>66.601399200000003</v>
       </c>
       <c r="L71">
         <v>3003.36</v>
       </c>
       <c r="M71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.995076077873875</v>
       </c>
     </row>
@@ -6442,26 +6752,30 @@
         <v>75.567001000000005</v>
       </c>
       <c r="F72">
+        <f t="shared" si="10"/>
+        <v>63.080307265268658</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="6"/>
+        <v>61.459409693158698</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="7"/>
+        <v>73.154944973931137</v>
+      </c>
+      <c r="J72">
         <f t="shared" si="8"/>
-        <v>63.080307265268658</v>
-      </c>
-      <c r="G72">
-        <f t="shared" si="5"/>
-        <v>61.459409693158698</v>
-      </c>
-      <c r="H72">
-        <f t="shared" si="6"/>
-        <v>73.154944973931137</v>
-      </c>
-      <c r="J72">
-        <f t="shared" si="7"/>
         <v>119.27668979987615</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="9"/>
+        <v>65.248899800000004</v>
       </c>
       <c r="L72">
         <v>2999.62</v>
       </c>
       <c r="M72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.901686812340841</v>
       </c>
     </row>
@@ -6479,26 +6793,30 @@
         <v>76.028998999999999</v>
       </c>
       <c r="F73">
+        <f t="shared" si="10"/>
+        <v>62.053421052878271</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="6"/>
+        <v>61.857979154175993</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="7"/>
+        <v>72.710411457607123</v>
+      </c>
+      <c r="J73">
         <f t="shared" si="8"/>
-        <v>62.053421052878271</v>
-      </c>
-      <c r="G73">
-        <f t="shared" si="5"/>
-        <v>61.857979154175993</v>
-      </c>
-      <c r="H73">
-        <f t="shared" si="6"/>
-        <v>72.710411457607123</v>
-      </c>
-      <c r="J73">
-        <f t="shared" si="7"/>
         <v>119.09506432875197</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="9"/>
+        <v>65.457299800000001</v>
       </c>
       <c r="L73">
         <v>2989.3</v>
       </c>
       <c r="M73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.643992368410167</v>
       </c>
     </row>
@@ -6516,26 +6834,30 @@
         <v>75.681999000000005</v>
       </c>
       <c r="F74">
+        <f t="shared" si="10"/>
+        <v>61.629575065327664</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="6"/>
+        <v>63.402542417636035</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="7"/>
+        <v>73.043786805895536</v>
+      </c>
+      <c r="J74">
         <f t="shared" si="8"/>
-        <v>61.629575065327664</v>
-      </c>
-      <c r="G74">
-        <f t="shared" si="5"/>
-        <v>63.402542417636035</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="6"/>
-        <v>73.043786805895536</v>
-      </c>
-      <c r="J74">
-        <f t="shared" si="7"/>
         <v>117.06385106309276</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="9"/>
+        <v>64.770098800000014</v>
       </c>
       <c r="L74">
         <v>2965.52</v>
       </c>
       <c r="M74">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.050196450128027</v>
       </c>
     </row>
@@ -6553,26 +6875,30 @@
         <v>75.900002000000001</v>
       </c>
       <c r="F75">
+        <f t="shared" si="10"/>
+        <v>62.397370171694334</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="6"/>
+        <v>63.592123190510463</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="7"/>
+        <v>72.833987540606373</v>
+      </c>
+      <c r="J75">
         <f t="shared" si="8"/>
-        <v>62.397370171694334</v>
-      </c>
-      <c r="G75">
-        <f t="shared" si="5"/>
-        <v>63.592123190510463</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="6"/>
-        <v>72.833987540606373</v>
-      </c>
-      <c r="J75">
-        <f t="shared" si="7"/>
         <v>116.54423878366396</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="9"/>
+        <v>64.483499199999997</v>
       </c>
       <c r="L75">
         <v>2979.77</v>
       </c>
       <c r="M75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.406024534043937</v>
       </c>
     </row>
@@ -6590,26 +6916,30 @@
         <v>75.777495999999999</v>
       </c>
       <c r="F76">
+        <f t="shared" si="10"/>
+        <v>62.523683917092001</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="6"/>
+        <v>64.406462739543699</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="7"/>
+        <v>72.951734905571428</v>
+      </c>
+      <c r="J76">
         <f t="shared" si="8"/>
-        <v>62.523683917092001</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="5"/>
-        <v>64.406462739543699</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="6"/>
-        <v>72.951734905571428</v>
-      </c>
-      <c r="J76">
-        <f t="shared" si="7"/>
         <v>115.40904874237957</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="9"/>
+        <v>64.040698000000006</v>
       </c>
       <c r="L76">
         <v>2984.25</v>
       </c>
       <c r="M76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.517891889548736</v>
       </c>
     </row>
@@ -6627,26 +6957,30 @@
         <v>78.286002999999994</v>
       </c>
       <c r="F77">
+        <f t="shared" si="10"/>
+        <v>61.233258495452937</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="6"/>
+        <v>59.674556739610267</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="7"/>
+        <v>70.614153081745656</v>
+      </c>
+      <c r="J77">
         <f t="shared" si="8"/>
-        <v>61.233258495452937</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="5"/>
-        <v>59.674556739610267</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="6"/>
-        <v>70.614153081745656</v>
-      </c>
-      <c r="J77">
-        <f t="shared" si="7"/>
         <v>122.89492276991348</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="9"/>
+        <v>67.297099200000005</v>
       </c>
       <c r="L77">
         <v>2978.08</v>
       </c>
       <c r="M77">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.363824571811108</v>
       </c>
     </row>
@@ -6664,26 +6998,30 @@
         <v>77.920997999999997</v>
       </c>
       <c r="F78">
+        <f t="shared" si="10"/>
+        <v>62.090207216494804</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="6"/>
+        <v>60.787880636018961</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="7"/>
+        <v>70.944930659127323</v>
+      </c>
+      <c r="J78">
         <f t="shared" si="8"/>
-        <v>62.090207216494804</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="5"/>
-        <v>60.787880636018961</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="6"/>
-        <v>70.944930659127323</v>
-      </c>
-      <c r="J78">
-        <f t="shared" si="7"/>
         <v>120.85157689926571</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="9"/>
+        <v>66.367100600000001</v>
       </c>
       <c r="L78">
         <v>2964.66</v>
       </c>
       <c r="M78">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.028721913133808</v>
       </c>
     </row>
@@ -6701,26 +7039,30 @@
         <v>78.424499999999995</v>
       </c>
       <c r="F79">
+        <f t="shared" si="10"/>
+        <v>61.916267824063979</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="6"/>
+        <v>61.540498024397472</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="7"/>
+        <v>70.489449087976325</v>
+      </c>
+      <c r="J79">
         <f t="shared" si="8"/>
-        <v>61.916267824063979</v>
-      </c>
-      <c r="G79">
-        <f t="shared" si="5"/>
-        <v>61.540498024397472</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="6"/>
-        <v>70.489449087976325</v>
-      </c>
-      <c r="J79">
-        <f t="shared" si="7"/>
         <v>119.85740895825823</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="9"/>
+        <v>66.138499600000003</v>
       </c>
       <c r="L79">
         <v>2971.41</v>
       </c>
       <c r="M79">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74.197272058146609</v>
       </c>
     </row>
@@ -6738,26 +7080,30 @@
         <v>75.783996999999999</v>
       </c>
       <c r="F80">
+        <f t="shared" si="10"/>
+        <v>64.868867845668888</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="6"/>
+        <v>63.876380866728375</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="7"/>
+        <v>72.945476866309903</v>
+      </c>
+      <c r="J80">
         <f t="shared" si="8"/>
-        <v>64.868867845668888</v>
-      </c>
-      <c r="G80">
-        <f t="shared" si="5"/>
-        <v>63.876380866728375</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="6"/>
-        <v>72.945476866309903</v>
-      </c>
-      <c r="J80">
-        <f t="shared" si="7"/>
         <v>115.30542925053362</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="9"/>
+        <v>63.591299399999997</v>
       </c>
       <c r="L80">
         <v>2932.94</v>
       </c>
       <c r="M80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>73.236661083532908</v>
       </c>
     </row>
@@ -6775,26 +7121,30 @@
         <v>75.593497999999997</v>
       </c>
       <c r="F81">
+        <f t="shared" si="10"/>
+        <v>65.029965233060807</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="6"/>
+        <v>63.401699975119236</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="7"/>
+        <v>73.129302734475914</v>
+      </c>
+      <c r="J81">
         <f t="shared" si="8"/>
-        <v>65.029965233060807</v>
-      </c>
-      <c r="G81">
-        <f t="shared" si="5"/>
-        <v>63.401699975119236</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="6"/>
-        <v>73.129302734475914</v>
-      </c>
-      <c r="J81">
-        <f t="shared" si="7"/>
         <v>115.88043140254155</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="9"/>
+        <v>63.730798399999998</v>
       </c>
       <c r="L81">
         <v>2919.66</v>
       </c>
       <c r="M81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>72.905054279715131</v>
       </c>
     </row>
@@ -6812,26 +7162,30 @@
         <v>76.510002</v>
       </c>
       <c r="F82">
+        <f t="shared" si="10"/>
+        <v>63.524419650341066</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="6"/>
+        <v>62.440881804404697</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="7"/>
+        <v>72.253295719427626</v>
+      </c>
+      <c r="J82">
         <f t="shared" si="8"/>
-        <v>63.524419650341066</v>
-      </c>
-      <c r="G82">
-        <f t="shared" si="5"/>
-        <v>62.440881804404697</v>
-      </c>
-      <c r="H82">
-        <f t="shared" si="6"/>
-        <v>72.253295719427626</v>
-      </c>
-      <c r="J82">
-        <f t="shared" si="7"/>
         <v>117.80556408552548</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="9"/>
+        <v>64.816099600000001</v>
       </c>
       <c r="L82">
         <v>2926.07</v>
       </c>
       <c r="M82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>73.065114491497667</v>
       </c>
     </row>
@@ -6849,26 +7203,30 @@
         <v>75.016998000000001</v>
       </c>
       <c r="F83">
+        <f t="shared" si="10"/>
+        <v>64.585399542416525</v>
+      </c>
+      <c r="G83">
+        <f t="shared" ref="G83:G86" si="12">G82*C82/C83</f>
+        <v>63.583009321741592</v>
+      </c>
+      <c r="H83">
+        <f t="shared" ref="H83:H86" si="13">H82*D82/D83</f>
+        <v>73.691295938021923</v>
+      </c>
+      <c r="J83">
         <f t="shared" si="8"/>
-        <v>64.585399542416525</v>
-      </c>
-      <c r="G83">
-        <f t="shared" ref="G83:G86" si="10">G82*C82/C83</f>
-        <v>63.583009321741592</v>
-      </c>
-      <c r="H83">
-        <f t="shared" ref="H83:H86" si="11">H82*D82/D83</f>
-        <v>73.691295938021923</v>
-      </c>
-      <c r="J83">
-        <f t="shared" si="7"/>
         <v>115.708917353643</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="9"/>
+        <v>63.657198999999999</v>
       </c>
       <c r="L83">
         <v>2945.78</v>
       </c>
       <c r="M83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>73.557280914935049</v>
       </c>
     </row>
@@ -6886,26 +7244,30 @@
         <v>76.100998000000004</v>
       </c>
       <c r="F84">
+        <f t="shared" si="10"/>
+        <v>63.370686412345435</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="12"/>
+        <v>62.887133641495332</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="13"/>
+        <v>72.641620284664313</v>
+      </c>
+      <c r="J84">
         <f t="shared" si="8"/>
-        <v>63.370686412345435</v>
-      </c>
-      <c r="G84">
-        <f t="shared" si="10"/>
-        <v>62.887133641495332</v>
-      </c>
-      <c r="H84">
-        <f t="shared" si="11"/>
-        <v>72.641620284664313</v>
-      </c>
-      <c r="J84">
-        <f t="shared" si="7"/>
         <v>117.18610076522592</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="9"/>
+        <v>64.563499400000012</v>
       </c>
       <c r="L84">
         <v>2951.42</v>
       </c>
       <c r="M84">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>73.698113924990196</v>
       </c>
     </row>
@@ -6923,26 +7285,30 @@
         <v>76.572502</v>
       </c>
       <c r="F85">
+        <f t="shared" si="10"/>
+        <v>62.613057228130593</v>
+      </c>
+      <c r="G85">
+        <f t="shared" si="12"/>
+        <v>62.509014607744</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="13"/>
+        <v>72.194321141550247</v>
+      </c>
+      <c r="J85">
         <f t="shared" si="8"/>
-        <v>62.613057228130593</v>
-      </c>
-      <c r="G85">
-        <f t="shared" si="10"/>
-        <v>62.509014607744</v>
-      </c>
-      <c r="H85">
-        <f t="shared" si="11"/>
-        <v>72.194321141550247</v>
-      </c>
-      <c r="J85">
-        <f t="shared" si="7"/>
         <v>118.02681608704816</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="9"/>
+        <v>65.071299600000003</v>
       </c>
       <c r="L85">
         <v>2952.71</v>
       </c>
       <c r="M85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>73.730325730481539</v>
       </c>
     </row>
@@ -6960,26 +7326,30 @@
         <v>74.148003000000003</v>
       </c>
       <c r="F86">
+        <f t="shared" si="10"/>
+        <v>56.679371227566854</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="12"/>
+        <v>60.280979825359147</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="13"/>
+        <v>74.554938451949937</v>
+      </c>
+      <c r="J86">
         <f t="shared" si="8"/>
-        <v>56.679371227566854</v>
-      </c>
-      <c r="G86">
-        <f t="shared" si="10"/>
-        <v>60.280979825359147</v>
-      </c>
-      <c r="H86">
-        <f t="shared" si="11"/>
-        <v>74.554938451949937</v>
-      </c>
-      <c r="J86">
-        <f t="shared" si="7"/>
         <v>123.51424617925211</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="9"/>
+        <v>67.728399800000005</v>
       </c>
       <c r="L86">
         <v>2949.6</v>
       </c>
       <c r="M86">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>73.652667811816372</v>
       </c>
     </row>
@@ -9495,4 +9865,124 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4754E949-CAE8-4BA8-BA5A-3B7CADC8F5D7}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="9">
+        <v>44858</v>
+      </c>
+      <c r="B1" s="10">
+        <v>149.449997</v>
+      </c>
+      <c r="C1" s="10">
+        <v>119.82</v>
+      </c>
+      <c r="D1" s="10">
+        <v>102.970001</v>
+      </c>
+      <c r="E1" s="10">
+        <v>129.720001</v>
+      </c>
+      <c r="F1">
+        <f>0.2*B1+0.2*C1+0.2*D1+0.2*E1</f>
+        <v>100.39199980000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>44859</v>
+      </c>
+      <c r="B2" s="10">
+        <v>152.33999600000001</v>
+      </c>
+      <c r="C2" s="10">
+        <v>120.599998</v>
+      </c>
+      <c r="D2" s="10">
+        <v>104.93</v>
+      </c>
+      <c r="E2" s="10">
+        <v>137.509995</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F5" si="0">0.2*B2+0.2*C2+0.2*D2+0.2*E2</f>
+        <v>103.07599780000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>44860</v>
+      </c>
+      <c r="B3" s="10">
+        <v>149.35000600000001</v>
+      </c>
+      <c r="C3" s="10">
+        <v>115.660004</v>
+      </c>
+      <c r="D3" s="10">
+        <v>94.82</v>
+      </c>
+      <c r="E3" s="10">
+        <v>129.820007</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>97.930003400000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>44861</v>
+      </c>
+      <c r="B4" s="10">
+        <v>144.800003</v>
+      </c>
+      <c r="C4" s="10">
+        <v>110.959999</v>
+      </c>
+      <c r="D4" s="10">
+        <v>92.599997999999999</v>
+      </c>
+      <c r="E4" s="10">
+        <v>97.940002000000007</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>89.26000040000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>44862</v>
+      </c>
+      <c r="B5" s="10">
+        <v>155.740005</v>
+      </c>
+      <c r="C5" s="10">
+        <v>103.410004</v>
+      </c>
+      <c r="D5" s="10">
+        <v>96.580001999999993</v>
+      </c>
+      <c r="E5" s="10">
+        <v>99.199996999999996</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>90.986001599999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>